<commit_message>
add gender to partenaire database
</commit_message>
<xml_diff>
--- a/data/ANR_CES_list.xlsx
+++ b/data/ANR_CES_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/analutzky/Desktop/SICSS_2002/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomd\Documents\MEGA\github\ANR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BB8E4C-320B-B047-8440-4A3B20FD8847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21A8331-3A08-4221-AA01-5D06D04A3843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8620" yWindow="2200" windowWidth="13760" windowHeight="15800" xr2:uid="{33BE1310-DC2A-4F45-967E-230EA85E0BEA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{33BE1310-DC2A-4F45-967E-230EA85E0BEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil2" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="184">
   <si>
     <t xml:space="preserve">Terre solide et enveloppes fluides </t>
   </si>
@@ -548,6 +548,45 @@
   </si>
   <si>
     <t>H.9</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>Environnemental science</t>
+  </si>
+  <si>
+    <t>Physique</t>
+  </si>
+  <si>
+    <t>Social Sciences</t>
+  </si>
+  <si>
+    <t>Physics</t>
+  </si>
+  <si>
+    <t>Biology</t>
+  </si>
+  <si>
+    <t>Chemestry</t>
+  </si>
+  <si>
+    <t>Medecine</t>
+  </si>
+  <si>
+    <t>Geography</t>
+  </si>
+  <si>
+    <t>Computational Science</t>
+  </si>
+  <si>
+    <t>Neurosciences</t>
+  </si>
+  <si>
+    <t>Mathematics</t>
+  </si>
+  <si>
+    <t>Engineering</t>
   </si>
 </sst>
 </file>
@@ -905,18 +944,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD91035-84D6-D24E-A981-102F48610E46}">
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -926,8 +966,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -937,8 +980,11 @@
       <c r="C2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -948,8 +994,11 @@
       <c r="C3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>134</v>
       </c>
@@ -959,8 +1008,11 @@
       <c r="C4" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>162</v>
       </c>
@@ -970,8 +1022,11 @@
       <c r="C5" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>170</v>
       </c>
@@ -981,8 +1036,11 @@
       <c r="C6" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>88</v>
       </c>
@@ -992,8 +1050,11 @@
       <c r="C7" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>94</v>
       </c>
@@ -1003,8 +1064,11 @@
       <c r="C8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>90</v>
       </c>
@@ -1014,8 +1078,11 @@
       <c r="C9" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>136</v>
       </c>
@@ -1025,8 +1092,11 @@
       <c r="C10" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>154</v>
       </c>
@@ -1036,8 +1106,11 @@
       <c r="C11" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>103</v>
       </c>
@@ -1047,8 +1120,11 @@
       <c r="C12" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>105</v>
       </c>
@@ -1058,8 +1134,11 @@
       <c r="C13" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>107</v>
       </c>
@@ -1069,8 +1148,11 @@
       <c r="C14" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>108</v>
       </c>
@@ -1080,8 +1162,11 @@
       <c r="C15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>110</v>
       </c>
@@ -1091,8 +1176,11 @@
       <c r="C16" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>112</v>
       </c>
@@ -1102,8 +1190,11 @@
       <c r="C17" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>115</v>
       </c>
@@ -1113,8 +1204,11 @@
       <c r="C18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -1124,8 +1218,11 @@
       <c r="C19" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>141</v>
       </c>
@@ -1135,8 +1232,11 @@
       <c r="C20" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -1146,8 +1246,11 @@
       <c r="C21" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -1157,8 +1260,11 @@
       <c r="C22" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>152</v>
       </c>
@@ -1168,8 +1274,11 @@
       <c r="C23" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>119</v>
       </c>
@@ -1179,8 +1288,11 @@
       <c r="C24" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>140</v>
       </c>
@@ -1190,8 +1302,11 @@
       <c r="C25" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>121</v>
       </c>
@@ -1201,8 +1316,11 @@
       <c r="C26" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>65</v>
       </c>
@@ -1212,8 +1330,11 @@
       <c r="C27" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -1223,8 +1344,11 @@
       <c r="C28" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -1234,8 +1358,11 @@
       <c r="C29" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>96</v>
       </c>
@@ -1245,8 +1372,11 @@
       <c r="C30" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -1256,8 +1386,11 @@
       <c r="C31" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>132</v>
       </c>
@@ -1267,8 +1400,11 @@
       <c r="C32" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>164</v>
       </c>
@@ -1278,8 +1414,11 @@
       <c r="C33" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>123</v>
       </c>
@@ -1289,8 +1428,11 @@
       <c r="C34" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>156</v>
       </c>
@@ -1300,8 +1442,11 @@
       <c r="C35" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>158</v>
       </c>
@@ -1311,8 +1456,11 @@
       <c r="C36" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>160</v>
       </c>
@@ -1322,8 +1470,11 @@
       <c r="C37" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>114</v>
       </c>
@@ -1333,8 +1484,11 @@
       <c r="C38" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>145</v>
       </c>
@@ -1344,8 +1498,11 @@
       <c r="C39" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>150</v>
       </c>
@@ -1355,8 +1512,11 @@
       <c r="C40" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>128</v>
       </c>
@@ -1366,8 +1526,11 @@
       <c r="C41" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>67</v>
       </c>
@@ -1377,8 +1540,11 @@
       <c r="C42" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>138</v>
       </c>
@@ -1388,8 +1554,11 @@
       <c r="C43" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>166</v>
       </c>
@@ -1399,8 +1568,11 @@
       <c r="C44" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>97</v>
       </c>
@@ -1410,8 +1582,11 @@
       <c r="C45" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>143</v>
       </c>
@@ -1421,8 +1596,11 @@
       <c r="C46" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>125</v>
       </c>
@@ -1432,8 +1610,11 @@
       <c r="C47" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>126</v>
       </c>
@@ -1443,8 +1624,11 @@
       <c r="C48" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>117</v>
       </c>
@@ -1454,8 +1638,11 @@
       <c r="C49" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>130</v>
       </c>
@@ -1465,8 +1652,11 @@
       <c r="C50" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>168</v>
       </c>
@@ -1476,8 +1666,11 @@
       <c r="C51" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>92</v>
       </c>
@@ -1487,8 +1680,11 @@
       <c r="C52" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>101</v>
       </c>
@@ -1498,8 +1694,11 @@
       <c r="C53" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>64</v>
       </c>
@@ -1509,8 +1708,11 @@
       <c r="C54" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>72</v>
       </c>
@@ -1520,8 +1722,11 @@
       <c r="C55" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>77</v>
       </c>
@@ -1531,8 +1736,11 @@
       <c r="C56" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>148</v>
       </c>
@@ -1541,6 +1749,9 @@
       </c>
       <c r="C57" t="s">
         <v>146</v>
+      </c>
+      <c r="D57" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add database on gender
</commit_message>
<xml_diff>
--- a/data/ANR_CES_list.xlsx
+++ b/data/ANR_CES_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomd\Documents\MEGA\github\ANR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21A8331-3A08-4221-AA01-5D06D04A3843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52940E5-E32D-41EA-A856-0490C1B8DEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{33BE1310-DC2A-4F45-967E-230EA85E0BEA}"/>
   </bookViews>
@@ -946,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD91035-84D6-D24E-A981-102F48610E46}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>